<commit_message>
file test to modified
</commit_message>
<xml_diff>
--- a/others/dev-shapley/bootstrap_exact.xlsx
+++ b/others/dev-shapley/bootstrap_exact.xlsx
@@ -419,13 +419,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.104644152585439</v>
+        <v>0.104813269303049</v>
       </c>
       <c r="C2">
-        <v>0.09301224370722315</v>
+        <v>0.09585042201537033</v>
       </c>
       <c r="D2">
-        <v>0.1115105953569688</v>
+        <v>0.1092849281569675</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -433,13 +433,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.416453107139893</v>
+        <v>0.4171261421903749</v>
       </c>
       <c r="C3">
-        <v>0.4080272493427919</v>
+        <v>0.4149373803962081</v>
       </c>
       <c r="D3">
-        <v>0.4262106643004804</v>
+        <v>0.4209267934553773</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -447,13 +447,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.47728923543187</v>
+        <v>0.4780605885065762</v>
       </c>
       <c r="C4">
-        <v>0.4694946703564503</v>
+        <v>0.4751933081685998</v>
       </c>
       <c r="D4">
-        <v>0.4876457423042979</v>
+        <v>0.483669597729377</v>
       </c>
     </row>
   </sheetData>
@@ -485,13 +485,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1063662255113449</v>
+        <v>0.1049220128443874</v>
       </c>
       <c r="C2">
-        <v>0.09014525607381627</v>
+        <v>0.07138096436810831</v>
       </c>
       <c r="D2">
-        <v>0.1052345431486882</v>
+        <v>0.1214878237641213</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -499,13 +499,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.8158777614347512</v>
+        <v>0.8155801991930413</v>
       </c>
       <c r="C3">
-        <v>0.812549518086061</v>
+        <v>0.8088032668573277</v>
       </c>
       <c r="D3">
-        <v>0.8156171469098823</v>
+        <v>0.8189034807945491</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -513,13 +513,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.876420215952106</v>
+        <v>0.8762204971247777</v>
       </c>
       <c r="C4">
-        <v>0.8741515933354043</v>
+        <v>0.8714746624616878</v>
       </c>
       <c r="D4">
-        <v>0.8763078926408476</v>
+        <v>0.878456829485212</v>
       </c>
     </row>
   </sheetData>
@@ -551,13 +551,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.104888600801009</v>
+        <v>0.1050581125744231</v>
       </c>
       <c r="C2">
-        <v>0.105036202663669</v>
+        <v>0.1031826900439379</v>
       </c>
       <c r="D2">
-        <v>0.1068251954525541</v>
+        <v>0.1091002248472033</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -565,13 +565,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.01970588443287419</v>
+        <v>0.01973773135800618</v>
       </c>
       <c r="C3">
-        <v>0.01972175389804536</v>
+        <v>0.01936216511791973</v>
       </c>
       <c r="D3">
-        <v>0.02007903664349004</v>
+        <v>0.02048436930152382</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -579,13 +579,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.0792542911841204</v>
+        <v>0.0793823750306652</v>
       </c>
       <c r="C4">
-        <v>0.07935364359533119</v>
+        <v>0.07788345051162671</v>
       </c>
       <c r="D4">
-        <v>0.08075190240950643</v>
+        <v>0.08247574127698191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>